<commit_message>
Report completed and Readme.txt added
</commit_message>
<xml_diff>
--- a/Instances Structure and Experiments.xlsx
+++ b/Instances Structure and Experiments.xlsx
@@ -187,13 +187,12 @@
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -212,11 +211,87 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -224,15 +299,56 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFE2EFDA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFFCE4D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FFA6A6A6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -261,19 +377,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA6A6A6"/>
         <bgColor rgb="FF9BC2E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FFA6A6A6"/>
       </patternFill>
     </fill>
     <fill>
@@ -285,13 +395,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF404040"/>
-        <bgColor rgb="FF333300"/>
+        <bgColor rgb="FF333333"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF4B084"/>
-        <bgColor rgb="FFFF8080"/>
+        <bgColor rgb="FFFFCCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -331,12 +441,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -347,7 +472,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -371,21 +496,72 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -397,35 +573,43 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -433,63 +617,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -501,91 +677,91 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="20" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="21" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="22" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -593,44 +769,61 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="23" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="23" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFF2F2F2"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFD0CECE"/>
       <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFF2F2F2"/>
+      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFDDEBF7"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -645,17 +838,17 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FFE2EFDA"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFE699"/>
       <rgbColor rgb="FF9BC2E6"/>
-      <rgbColor rgb="FFFCE4D6"/>
-      <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF4B084"/>
+      <rgbColor rgb="FFD9D9D9"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFCE4D6"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF595959"/>
@@ -663,11 +856,11 @@
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF70AD47"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF404040"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF404040"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -716,8 +909,8 @@
   </sheetPr>
   <dimension ref="E1:R410"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A350" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I369" activeCellId="0" sqref="I369"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10871,8 +11064,8 @@
         <v>45.036</v>
       </c>
       <c r="J274" s="29" t="n">
-        <f aca="false">AVERAGE(K269:K273)</f>
-        <v>2.2338</v>
+        <f aca="false">AVERAGE(J269:J273)</f>
+        <v>29.7136</v>
       </c>
       <c r="K274" s="29" t="n">
         <f aca="false">AVERAGE(K269:K273)</f>

</xml_diff>